<commit_message>
Updated the run time
</commit_message>
<xml_diff>
--- a/tables/RQ1_Table1.xlsx
+++ b/tables/RQ1_Table1.xlsx
@@ -436,104 +436,104 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>model</t>
+          <t>Model</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>accuracy</t>
+          <t>Accuracy</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>precision</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>recall</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>f1</t>
+          <t>F1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Multi-Source LR</t>
+          <t>Multi LR</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9714285714285714</v>
+        <v>0.971</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9702380952380952</v>
+        <v>0.97</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9939024390243902</v>
+        <v>0.994</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9819277108433735</v>
+        <v>0.982</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Multi-Source RF</t>
+          <t>Multi RF</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9476190476190476</v>
+        <v>0.948</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9636363636363636</v>
+        <v>0.964</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9695121951219512</v>
+        <v>0.97</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9665653495440729</v>
+        <v>0.967</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Single-Source LR</t>
+          <t>Single LR</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.929</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9461077844311377</v>
+        <v>0.946</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9634146341463414</v>
+        <v>0.963</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9546827794561934</v>
+        <v>0.955</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Single-Source RF</t>
+          <t>Single RF</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9142857142857143</v>
+        <v>0.914</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9397590361445783</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9512195121951219</v>
+        <v>0.951</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9454545454545454</v>
+        <v>0.945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>